<commit_message>
Dodani alternativni tokovi za registraciju korisnika
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/Registracija korisnika tok dogadjaja.xlsx
+++ b/UseCaseIScenarij/Registracija korisnika tok dogadjaja.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Registracij korisnika(sistem)</t>
   </si>
@@ -96,6 +96,64 @@
   </si>
   <si>
     <t>Alternativni tok  1:</t>
+  </si>
+  <si>
+    <t>Alternativni tok 2:</t>
+  </si>
+  <si>
+    <t>Na koraku 8 nije unesena validna lozinka, korisnik odustaje od registracije</t>
+  </si>
+  <si>
+    <t>Alternativni tok 3:</t>
+  </si>
+  <si>
+    <t>1. Nije uneseno validno ime (sadrži nevalidne karaktere)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Korisniku se nudi mogućnost 
+ponovnog unosa </t>
+  </si>
+  <si>
+    <t>4. Nastavak na koraku 2</t>
+  </si>
+  <si>
+    <t>Alternativni korak 4:</t>
+  </si>
+  <si>
+    <t>1. Nije uneseno validno korisničko ime (sadrži nevalidne karaktere)</t>
+  </si>
+  <si>
+    <t>Na koraku 6  nije uneseno validno korisničko ime</t>
+  </si>
+  <si>
+    <t>4. Nastavak na koraku 6</t>
+  </si>
+  <si>
+    <t>Na koraku 2 nije uneseno validno ime (analogno i za prezime, s tim da se vraća na korak 4.)</t>
+  </si>
+  <si>
+    <t>Alternativni korak 5:</t>
+  </si>
+  <si>
+    <t>Na koraku 10 nije unesen validan datum rođenja</t>
+  </si>
+  <si>
+    <t>1. Nije unesen validan datum</t>
+  </si>
+  <si>
+    <t>4. Nastavak na koraku 10</t>
+  </si>
+  <si>
+    <t>Alternativni korak 6:</t>
+  </si>
+  <si>
+    <t>Na koraku 12 nije unesen validan email</t>
+  </si>
+  <si>
+    <t>1. Nije unesen validan email</t>
+  </si>
+  <si>
+    <t>4. Nastavak na koraku 12</t>
   </si>
 </sst>
 </file>
@@ -167,6 +225,61 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="A15:B19" totalsRowShown="0">
   <autoFilter ref="A15:B19"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Neregistrovani korisnik"/>
+    <tableColumn id="2" name="Registracij korisnika(sistem)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle33" displayName="Tabelle33" ref="A24:B27" totalsRowShown="0">
+  <autoFilter ref="A24:B27"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Neregistrovani korisnik"/>
+    <tableColumn id="2" name="Registracij korisnika(sistem)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabelle335" displayName="Tabelle335" ref="A31:B35" totalsRowShown="0">
+  <autoFilter ref="A31:B35"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Neregistrovani korisnik"/>
+    <tableColumn id="2" name="Registracij korisnika(sistem)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabelle5" displayName="Tabelle5" ref="A39:B43" totalsRowShown="0">
+  <autoFilter ref="A39:B43"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Neregistrovani korisnik"/>
+    <tableColumn id="2" name="Registracij korisnika(sistem)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabelle58" displayName="Tabelle58" ref="A48:B52" totalsRowShown="0">
+  <autoFilter ref="A48:B52"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Neregistrovani korisnik"/>
+    <tableColumn id="2" name="Registracij korisnika(sistem)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabelle589" displayName="Tabelle589" ref="A56:B60" totalsRowShown="0">
+  <autoFilter ref="A56:B60"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Neregistrovani korisnik"/>
     <tableColumn id="2" name="Registracij korisnika(sistem)"/>
@@ -438,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,12 +672,202 @@
         <v>21</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="7">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>